<commit_message>
updating templates in this other location just in case
</commit_message>
<xml_diff>
--- a/frontend/public/bulk_import_templates/bulk_import_DO_template.xlsx
+++ b/frontend/public/bulk_import_templates/bulk_import_DO_template.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woodford/Documents/GitHub/archivesspace/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smith/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADCF748-4569-414A-BD02-5EDFE44EC6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FDA82B-3098-C34B-8B72-3EEB14E306B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7760" yWindow="6060" windowWidth="18440" windowHeight="11540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="27040" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Digital Object</t>
   </si>
   <si>
-    <t>digital_object_link</t>
-  </si>
-  <si>
     <t>ead</t>
   </si>
   <si>
@@ -79,30 +76,13 @@
     <t>Mapping - ArchivesSpace record FIELD with comments</t>
   </si>
   <si>
-    <t>Linked-to Digital Object URL 
-(Will set Actuate=onRequest, Show=new)</t>
-  </si>
-  <si>
-    <t>Thumbnail URL
-(Will set Actuate=onLoad, Show=embed)</t>
-  </si>
-  <si>
     <t>ao_ref_id</t>
   </si>
   <si>
-    <t>File URL of Linked-to digital object</t>
-  </si>
-  <si>
-    <t>File URL of Thumbnail</t>
-  </si>
-  <si>
     <t>ArchivesSpace digital object import field codes (please don't edit this row)</t>
   </si>
   <si>
     <t>publish</t>
-  </si>
-  <si>
-    <t>thumbnail</t>
   </si>
   <si>
     <t xml:space="preserve">Digital Object Identifier
@@ -144,13 +124,175 @@
   </si>
   <si>
     <t>Archival Object URI  REQUIRED IF NO REF ID</t>
+  </si>
+  <si>
+    <t>Linked-to URL for representative file version</t>
+  </si>
+  <si>
+    <t>Use Statement for representative file version</t>
+  </si>
+  <si>
+    <t>Xlink actuate attribute for representative file version (previous default 'onRequest')</t>
+  </si>
+  <si>
+    <t>Xlink show attribute for representative file version (previous default 'new')</t>
+  </si>
+  <si>
+    <t>File Format Name for representative file version</t>
+  </si>
+  <si>
+    <t>File Format Version for representative file version</t>
+  </si>
+  <si>
+    <t>File size (bytes) for representative file version</t>
+  </si>
+  <si>
+    <t>Checksum for representative file version</t>
+  </si>
+  <si>
+    <t>Checksum Method for representative file version</t>
+  </si>
+  <si>
+    <t>Caption for representative file version</t>
+  </si>
+  <si>
+    <t>Linked-to URL for non-representative file version</t>
+  </si>
+  <si>
+    <t>Publish non-representative file version?</t>
+  </si>
+  <si>
+    <t>Use Statement for non-representative file version</t>
+  </si>
+  <si>
+    <t>Xlink actuate attribute for non-representative file version (previous default 'onLoad')</t>
+  </si>
+  <si>
+    <t>Xlink show attribute for non-representative file version (previous default 'embed')</t>
+  </si>
+  <si>
+    <t>File Format Name for non-representative file version</t>
+  </si>
+  <si>
+    <t>File Format Version for non-representative file version</t>
+  </si>
+  <si>
+    <t>File size (bytes) for non-representative file version</t>
+  </si>
+  <si>
+    <t>Checksum for non-representative file version</t>
+  </si>
+  <si>
+    <t>Checksum Method for non-representative file version</t>
+  </si>
+  <si>
+    <t>Caption for non-representative file version</t>
+  </si>
+  <si>
+    <t>rep_use_statement</t>
+  </si>
+  <si>
+    <t>rep_xlink_actuate_attribute</t>
+  </si>
+  <si>
+    <t>rep_xlink_show_attribute</t>
+  </si>
+  <si>
+    <t>rep_file_format</t>
+  </si>
+  <si>
+    <t>rep_file_format_version</t>
+  </si>
+  <si>
+    <t>rep_file_size</t>
+  </si>
+  <si>
+    <t>rep_checksum</t>
+  </si>
+  <si>
+    <t>rep_checksum_method</t>
+  </si>
+  <si>
+    <t>rep_caption</t>
+  </si>
+  <si>
+    <t>nonrep_publish</t>
+  </si>
+  <si>
+    <t>nonrep_use_statement</t>
+  </si>
+  <si>
+    <t>nonrep_xlink_actuate_attribute</t>
+  </si>
+  <si>
+    <t>nonrep_xlink_show_attribute</t>
+  </si>
+  <si>
+    <t>nonrep_file_format</t>
+  </si>
+  <si>
+    <t>nonrep_file_format_version</t>
+  </si>
+  <si>
+    <t>nonrep_file_size</t>
+  </si>
+  <si>
+    <t>nonrep_checksum</t>
+  </si>
+  <si>
+    <t>nonrep_checksum_method</t>
+  </si>
+  <si>
+    <t>nonrep_caption</t>
+  </si>
+  <si>
+    <t>URL of representative file version</t>
+  </si>
+  <si>
+    <t>Publish</t>
+  </si>
+  <si>
+    <t>Use Statement</t>
+  </si>
+  <si>
+    <t>xlink actuate attribute</t>
+  </si>
+  <si>
+    <t>xlink show attribute</t>
+  </si>
+  <si>
+    <t>File Format Name</t>
+  </si>
+  <si>
+    <t>File Format Version</t>
+  </si>
+  <si>
+    <t>File Size</t>
+  </si>
+  <si>
+    <t>Checksum</t>
+  </si>
+  <si>
+    <t>Checksum Method</t>
+  </si>
+  <si>
+    <t>Caption</t>
+  </si>
+  <si>
+    <t>URL of non-representative file version</t>
+  </si>
+  <si>
+    <t>rep_file_uri</t>
+  </si>
+  <si>
+    <t>nonrep_file_uri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -204,8 +346,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +376,18 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6D9F1"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFE6E0EC"/>
       </patternFill>
     </fill>
   </fills>
@@ -319,18 +479,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -349,24 +503,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,9 +614,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -496,9 +654,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,26 +689,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,26 +724,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -776,16 +900,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ALJ6"/>
+  <dimension ref="A1:ALK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="10" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
@@ -794,160 +918,404 @@
     <col min="8" max="8" width="25.1640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.6640625" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5" style="1" customWidth="1"/>
-    <col min="12" max="998" width="9.33203125" style="1"/>
+    <col min="11" max="12" width="17.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" style="1" customWidth="1"/>
+    <col min="14" max="999" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" s="1" customFormat="1" ht="41.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD3" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="41.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>1</v>
+    <row r="4" spans="1:30" s="15" customFormat="1" ht="41.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="X4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y4" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA4" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC4" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD4" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="5" spans="1:30" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>20</v>
+      <c r="I5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="19" customFormat="1" ht="41.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>26</v>
-      </c>
+    <row r="6" spans="1:30" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="21"/>
     </row>
-    <row r="5" spans="1:11" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I1000 L1048555:L1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"FALSE,TRUE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R6:R1005 AC6" xr:uid="{E19F99B6-DD7B-4041-9C1B-21F2A327427A}">
+      <formula1>"MD5,SHA-1,SHA-256,SHA-384,SHA-512"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M6:M1005 X6:X1005" xr:uid="{E2D13213-7055-244F-8C8C-D708D6A65BFF}">
+      <formula1>"embed,new,none,other,replace"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L1005 W6:W1005" xr:uid="{A14C86AA-F54B-1E4D-A788-32DEB7EC3034}">
+      <formula1>"none,onLoad,onRequest,other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K1005 U6:U1005" xr:uid="{F30C24B7-91FF-3A47-B0B4-3C437D58D1D3}">
+      <formula1>"FALSE,TRUE"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
ANW-1734 Updates for file versions in AO/DO imports (#3087)
* Update templates in frontend/public/bulk_import_templates/ just in case
</commit_message>
<xml_diff>
--- a/frontend/public/bulk_import_templates/bulk_import_DO_template.xlsx
+++ b/frontend/public/bulk_import_templates/bulk_import_DO_template.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woodford/Documents/GitHub/archivesspace/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smith/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADCF748-4569-414A-BD02-5EDFE44EC6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FDA82B-3098-C34B-8B72-3EEB14E306B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7760" yWindow="6060" windowWidth="18440" windowHeight="11540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="27040" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Digital Object</t>
   </si>
   <si>
-    <t>digital_object_link</t>
-  </si>
-  <si>
     <t>ead</t>
   </si>
   <si>
@@ -79,30 +76,13 @@
     <t>Mapping - ArchivesSpace record FIELD with comments</t>
   </si>
   <si>
-    <t>Linked-to Digital Object URL 
-(Will set Actuate=onRequest, Show=new)</t>
-  </si>
-  <si>
-    <t>Thumbnail URL
-(Will set Actuate=onLoad, Show=embed)</t>
-  </si>
-  <si>
     <t>ao_ref_id</t>
   </si>
   <si>
-    <t>File URL of Linked-to digital object</t>
-  </si>
-  <si>
-    <t>File URL of Thumbnail</t>
-  </si>
-  <si>
     <t>ArchivesSpace digital object import field codes (please don't edit this row)</t>
   </si>
   <si>
     <t>publish</t>
-  </si>
-  <si>
-    <t>thumbnail</t>
   </si>
   <si>
     <t xml:space="preserve">Digital Object Identifier
@@ -144,13 +124,175 @@
   </si>
   <si>
     <t>Archival Object URI  REQUIRED IF NO REF ID</t>
+  </si>
+  <si>
+    <t>Linked-to URL for representative file version</t>
+  </si>
+  <si>
+    <t>Use Statement for representative file version</t>
+  </si>
+  <si>
+    <t>Xlink actuate attribute for representative file version (previous default 'onRequest')</t>
+  </si>
+  <si>
+    <t>Xlink show attribute for representative file version (previous default 'new')</t>
+  </si>
+  <si>
+    <t>File Format Name for representative file version</t>
+  </si>
+  <si>
+    <t>File Format Version for representative file version</t>
+  </si>
+  <si>
+    <t>File size (bytes) for representative file version</t>
+  </si>
+  <si>
+    <t>Checksum for representative file version</t>
+  </si>
+  <si>
+    <t>Checksum Method for representative file version</t>
+  </si>
+  <si>
+    <t>Caption for representative file version</t>
+  </si>
+  <si>
+    <t>Linked-to URL for non-representative file version</t>
+  </si>
+  <si>
+    <t>Publish non-representative file version?</t>
+  </si>
+  <si>
+    <t>Use Statement for non-representative file version</t>
+  </si>
+  <si>
+    <t>Xlink actuate attribute for non-representative file version (previous default 'onLoad')</t>
+  </si>
+  <si>
+    <t>Xlink show attribute for non-representative file version (previous default 'embed')</t>
+  </si>
+  <si>
+    <t>File Format Name for non-representative file version</t>
+  </si>
+  <si>
+    <t>File Format Version for non-representative file version</t>
+  </si>
+  <si>
+    <t>File size (bytes) for non-representative file version</t>
+  </si>
+  <si>
+    <t>Checksum for non-representative file version</t>
+  </si>
+  <si>
+    <t>Checksum Method for non-representative file version</t>
+  </si>
+  <si>
+    <t>Caption for non-representative file version</t>
+  </si>
+  <si>
+    <t>rep_use_statement</t>
+  </si>
+  <si>
+    <t>rep_xlink_actuate_attribute</t>
+  </si>
+  <si>
+    <t>rep_xlink_show_attribute</t>
+  </si>
+  <si>
+    <t>rep_file_format</t>
+  </si>
+  <si>
+    <t>rep_file_format_version</t>
+  </si>
+  <si>
+    <t>rep_file_size</t>
+  </si>
+  <si>
+    <t>rep_checksum</t>
+  </si>
+  <si>
+    <t>rep_checksum_method</t>
+  </si>
+  <si>
+    <t>rep_caption</t>
+  </si>
+  <si>
+    <t>nonrep_publish</t>
+  </si>
+  <si>
+    <t>nonrep_use_statement</t>
+  </si>
+  <si>
+    <t>nonrep_xlink_actuate_attribute</t>
+  </si>
+  <si>
+    <t>nonrep_xlink_show_attribute</t>
+  </si>
+  <si>
+    <t>nonrep_file_format</t>
+  </si>
+  <si>
+    <t>nonrep_file_format_version</t>
+  </si>
+  <si>
+    <t>nonrep_file_size</t>
+  </si>
+  <si>
+    <t>nonrep_checksum</t>
+  </si>
+  <si>
+    <t>nonrep_checksum_method</t>
+  </si>
+  <si>
+    <t>nonrep_caption</t>
+  </si>
+  <si>
+    <t>URL of representative file version</t>
+  </si>
+  <si>
+    <t>Publish</t>
+  </si>
+  <si>
+    <t>Use Statement</t>
+  </si>
+  <si>
+    <t>xlink actuate attribute</t>
+  </si>
+  <si>
+    <t>xlink show attribute</t>
+  </si>
+  <si>
+    <t>File Format Name</t>
+  </si>
+  <si>
+    <t>File Format Version</t>
+  </si>
+  <si>
+    <t>File Size</t>
+  </si>
+  <si>
+    <t>Checksum</t>
+  </si>
+  <si>
+    <t>Checksum Method</t>
+  </si>
+  <si>
+    <t>Caption</t>
+  </si>
+  <si>
+    <t>URL of non-representative file version</t>
+  </si>
+  <si>
+    <t>rep_file_uri</t>
+  </si>
+  <si>
+    <t>nonrep_file_uri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -204,8 +346,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +376,18 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6D9F1"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFE6E0EC"/>
       </patternFill>
     </fill>
   </fills>
@@ -319,18 +479,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -349,24 +503,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,9 +614,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -496,9 +654,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,26 +689,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,26 +724,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -776,16 +900,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ALJ6"/>
+  <dimension ref="A1:ALK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="10" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
@@ -794,160 +918,404 @@
     <col min="8" max="8" width="25.1640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.6640625" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5" style="1" customWidth="1"/>
-    <col min="12" max="998" width="9.33203125" style="1"/>
+    <col min="11" max="12" width="17.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" style="1" customWidth="1"/>
+    <col min="14" max="999" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" s="1" customFormat="1" ht="41.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD3" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="41.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>1</v>
+    <row r="4" spans="1:30" s="15" customFormat="1" ht="41.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="X4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y4" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA4" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC4" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD4" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="5" spans="1:30" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>20</v>
+      <c r="I5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="19" customFormat="1" ht="41.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>26</v>
-      </c>
+    <row r="6" spans="1:30" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="21"/>
     </row>
-    <row r="5" spans="1:11" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I1000 L1048555:L1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"FALSE,TRUE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R6:R1005 AC6" xr:uid="{E19F99B6-DD7B-4041-9C1B-21F2A327427A}">
+      <formula1>"MD5,SHA-1,SHA-256,SHA-384,SHA-512"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M6:M1005 X6:X1005" xr:uid="{E2D13213-7055-244F-8C8C-D708D6A65BFF}">
+      <formula1>"embed,new,none,other,replace"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L1005 W6:W1005" xr:uid="{A14C86AA-F54B-1E4D-A788-32DEB7EC3034}">
+      <formula1>"none,onLoad,onRequest,other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K1005 U6:U1005" xr:uid="{F30C24B7-91FF-3A47-B0B4-3C437D58D1D3}">
+      <formula1>"FALSE,TRUE"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
fix publish column name in DO import xslx
"publish" should be "digital_object_publish". Looks like I missed
this in the previous PR.
</commit_message>
<xml_diff>
--- a/frontend/public/bulk_import_templates/bulk_import_DO_template.xlsx
+++ b/frontend/public/bulk_import_templates/bulk_import_DO_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smith/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smith/work/projects/archivesspace/frontend/public/bulk_import_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FDA82B-3098-C34B-8B72-3EEB14E306B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891A0FE5-0B82-6F4D-8A98-259E2E3E6674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="27040" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>ArchivesSpace digital object import field codes (please don't edit this row)</t>
   </si>
   <si>
-    <t>publish</t>
-  </si>
-  <si>
     <t xml:space="preserve">Digital Object Identifier
 (Leave this blank to get a default system-assigned Digital Object Identifier that is based on the Archival Object Ref ID. Or enter a custom identifier here to override the default. Custom identifier must be unique within ArchivesSpace.  Note that Digital Object Identifiers are not exported in the EAD.)
 </t>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>nonrep_file_uri</t>
+  </si>
+  <si>
+    <t>digital_object_publish</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -925,7 +925,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="1" customFormat="1" ht="41.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1031,85 +1031,85 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="M3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="N3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="R3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="S3" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="T3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="U3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="19" t="s">
+      <c r="V3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="V3" s="19" t="s">
+      <c r="W3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="W3" s="19" t="s">
+      <c r="X3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="X3" s="19" t="s">
+      <c r="Y3" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="Y3" s="19" t="s">
+      <c r="Z3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="AA3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="AA3" s="19" t="s">
+      <c r="AB3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="AB3" s="19" t="s">
+      <c r="AC3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="AC3" s="19" t="s">
+      <c r="AD3" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="AD3" s="19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="15" customFormat="1" ht="41.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1123,13 +1123,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>16</v>
@@ -1138,70 +1138,70 @@
         <v>7</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="J4" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="S4" s="20" t="s">
+      <c r="U4" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="T4" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="U4" s="20" t="s">
+      <c r="V4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="V4" s="20" t="s">
+      <c r="W4" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="W4" s="20" t="s">
+      <c r="X4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="X4" s="20" t="s">
+      <c r="Y4" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="Y4" s="20" t="s">
+      <c r="Z4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="Z4" s="20" t="s">
+      <c r="AA4" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="AA4" s="20" t="s">
+      <c r="AB4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="AB4" s="20" t="s">
+      <c r="AC4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AC4" s="20" t="s">
+      <c r="AD4" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="AD4" s="20" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1215,13 +1215,13 @@
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>15</v>
@@ -1230,70 +1230,70 @@
         <v>12</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="V5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="W5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="AA5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="V5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="W5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="X5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD5" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="19" thickTop="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix publish column name in DO import xslx (#3122)
"publish" should be "digital_object_publish". Looks like I missed
this in the previous PR.
</commit_message>
<xml_diff>
--- a/frontend/public/bulk_import_templates/bulk_import_DO_template.xlsx
+++ b/frontend/public/bulk_import_templates/bulk_import_DO_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smith/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smith/work/projects/archivesspace/frontend/public/bulk_import_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FDA82B-3098-C34B-8B72-3EEB14E306B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891A0FE5-0B82-6F4D-8A98-259E2E3E6674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="27040" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>ArchivesSpace digital object import field codes (please don't edit this row)</t>
   </si>
   <si>
-    <t>publish</t>
-  </si>
-  <si>
     <t xml:space="preserve">Digital Object Identifier
 (Leave this blank to get a default system-assigned Digital Object Identifier that is based on the Archival Object Ref ID. Or enter a custom identifier here to override the default. Custom identifier must be unique within ArchivesSpace.  Note that Digital Object Identifiers are not exported in the EAD.)
 </t>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>nonrep_file_uri</t>
+  </si>
+  <si>
+    <t>digital_object_publish</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -925,7 +925,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="1" customFormat="1" ht="41.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1031,85 +1031,85 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="M3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="N3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="R3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="S3" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="T3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="U3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="19" t="s">
+      <c r="V3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="V3" s="19" t="s">
+      <c r="W3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="W3" s="19" t="s">
+      <c r="X3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="X3" s="19" t="s">
+      <c r="Y3" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="Y3" s="19" t="s">
+      <c r="Z3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="AA3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="AA3" s="19" t="s">
+      <c r="AB3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="AB3" s="19" t="s">
+      <c r="AC3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="AC3" s="19" t="s">
+      <c r="AD3" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="AD3" s="19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="15" customFormat="1" ht="41.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1123,13 +1123,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>16</v>
@@ -1138,70 +1138,70 @@
         <v>7</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="J4" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="S4" s="20" t="s">
+      <c r="U4" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="T4" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="U4" s="20" t="s">
+      <c r="V4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="V4" s="20" t="s">
+      <c r="W4" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="W4" s="20" t="s">
+      <c r="X4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="X4" s="20" t="s">
+      <c r="Y4" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="Y4" s="20" t="s">
+      <c r="Z4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="Z4" s="20" t="s">
+      <c r="AA4" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="AA4" s="20" t="s">
+      <c r="AB4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="AB4" s="20" t="s">
+      <c r="AC4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AC4" s="20" t="s">
+      <c r="AD4" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="AD4" s="20" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1215,13 +1215,13 @@
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>15</v>
@@ -1230,70 +1230,70 @@
         <v>12</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="V5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="W5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="AA5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="V5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="W5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="X5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD5" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="19" thickTop="1" x14ac:dyDescent="0.2">

</xml_diff>